<commit_message>
Worked on notebook and clean details
</commit_message>
<xml_diff>
--- a/data/quotation_princing_analysis/DRY BLENDING PROJECT PHASE 1 STRUCTURE - EDP.xlsx
+++ b/data/quotation_princing_analysis/DRY BLENDING PROJECT PHASE 1 STRUCTURE - EDP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\00_ML\00_Power BI\docu1\tbmc-data-management\data\quotation_princing_analysis\Ongoing\For CSV\for next cleaning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\00_ML\00_Power BI\docu1\tbmc-data-management\data\quotation_princing_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CB6E61-A227-4EF0-BDB0-B3C9C45F7EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997589CA-24FA-49EB-9A7D-A71263227EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,22 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="71">
-  <si>
-    <t>Man'r</t>
-  </si>
-  <si>
-    <t>UNIT</t>
-  </si>
-  <si>
-    <t>QTY</t>
-  </si>
-  <si>
-    <t>U/RATE</t>
-  </si>
-  <si>
-    <t>AMOUNT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="61">
   <si>
     <t>Mobilization/Demobilization &amp; Housekeeping</t>
   </si>
@@ -93,15 +78,6 @@
     <t>EDP</t>
   </si>
   <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>SOURCE</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
     <t>Materials</t>
   </si>
   <si>
@@ -111,13 +87,7 @@
     <t>Labor</t>
   </si>
   <si>
-    <t>PROJECT</t>
-  </si>
-  <si>
     <t>DRY BLENDING PROJECT PHASE-1  STRUCTURE</t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
   </si>
   <si>
     <t>mobilization/demobilization &amp; housekeeping</t>
@@ -688,10 +658,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -707,1219 +677,1218 @@
     <col min="11" max="16384" width="3.5546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13">
+        <v>10000</v>
+      </c>
+      <c r="F1" s="13">
+        <f>E1*D1</f>
+        <v>10000</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>18</v>
+      <c r="I1" s="4">
+        <v>45392</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="13">
-        <v>10000</v>
-      </c>
-      <c r="F2" s="13">
-        <f>E2*D2</f>
-        <v>10000</v>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1500</v>
+      </c>
+      <c r="F2" s="19">
+        <f t="shared" ref="F2:F43" si="0">D2*E2</f>
+        <v>1500</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I2" s="4">
         <v>45392</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D3" s="13">
         <v>1</v>
       </c>
-      <c r="E3" s="17">
-        <v>1500</v>
+      <c r="E3" s="13">
+        <v>4500</v>
       </c>
       <c r="F3" s="19">
-        <f t="shared" ref="F3:F44" si="0">D3*E3</f>
-        <v>1500</v>
+        <f t="shared" si="0"/>
+        <v>4500</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I3" s="4">
         <v>45392</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="13">
-        <v>1</v>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12">
+        <v>75</v>
       </c>
       <c r="E4" s="13">
-        <v>4500</v>
+        <v>50</v>
       </c>
       <c r="F4" s="19">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>3750</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I4" s="4">
         <v>45392</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D5" s="12">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="E5" s="13">
         <v>50</v>
       </c>
       <c r="F5" s="19">
         <f t="shared" si="0"/>
-        <v>3750</v>
+        <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I5" s="4">
         <v>45392</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B6" s="5"/>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D6" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="13">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="F6" s="19">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>4500</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I6" s="4">
         <v>45392</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D7" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="13">
-        <v>1500</v>
+        <v>250</v>
       </c>
       <c r="F7" s="19">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>250</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I7" s="4">
         <v>45392</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D8" s="12">
         <v>1</v>
       </c>
       <c r="E8" s="13">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="F8" s="19">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I8" s="4">
         <v>45392</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D9" s="12">
         <v>1</v>
       </c>
       <c r="E9" s="13">
-        <v>450</v>
+        <v>150</v>
       </c>
       <c r="F9" s="19">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>150</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I9" s="4">
         <v>45392</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="12">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13">
+        <v>3</v>
+      </c>
+      <c r="D10" s="13">
+        <v>5</v>
+      </c>
+      <c r="E10" s="15">
         <v>150</v>
       </c>
       <c r="F10" s="19">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>750</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I10" s="4">
         <v>45392</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D11" s="13">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="E11" s="15">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="F11" s="19">
         <f t="shared" si="0"/>
-        <v>750</v>
+        <v>6000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I11" s="4">
         <v>45392</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D12" s="13">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="E12" s="15">
-        <v>80</v>
+        <v>350</v>
       </c>
       <c r="F12" s="19">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>1750</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I12" s="4">
         <v>45392</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D13" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E13" s="15">
-        <v>350</v>
+        <v>650</v>
       </c>
       <c r="F13" s="19">
         <f t="shared" si="0"/>
-        <v>1750</v>
+        <v>650</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I13" s="4">
         <v>45392</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D14" s="13">
         <v>1</v>
       </c>
       <c r="E14" s="15">
-        <v>650</v>
+        <v>1000</v>
       </c>
       <c r="F14" s="19">
         <f t="shared" si="0"/>
-        <v>650</v>
+        <v>1000</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I14" s="4">
         <v>45392</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D15" s="13">
         <v>1</v>
       </c>
       <c r="E15" s="15">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="F15" s="19">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I15" s="4">
         <v>45392</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D16" s="13">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E16" s="15">
-        <v>3000</v>
+        <v>80</v>
       </c>
       <c r="F16" s="19">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I16" s="4">
         <v>45392</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D17" s="13">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E17" s="15">
-        <v>80</v>
+        <v>900</v>
       </c>
       <c r="F17" s="19">
         <f t="shared" si="0"/>
-        <v>2400</v>
+        <v>900</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I17" s="4">
         <v>45392</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18" s="13">
         <v>1</v>
       </c>
-      <c r="E18" s="15">
-        <v>900</v>
+      <c r="E18" s="17">
+        <v>6750</v>
       </c>
       <c r="F18" s="19">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>6750</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I18" s="4">
         <v>45392</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D19" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="17">
-        <v>6750</v>
+        <v>9750</v>
       </c>
       <c r="F19" s="19">
         <f t="shared" si="0"/>
-        <v>6750</v>
+        <v>19500</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I19" s="4">
         <v>45392</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D20" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="17">
-        <v>9750</v>
+        <v>4500</v>
       </c>
       <c r="F20" s="19">
         <f t="shared" si="0"/>
-        <v>19500</v>
+        <v>4500</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I20" s="4">
         <v>45392</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D21" s="13">
         <v>1</v>
       </c>
-      <c r="E21" s="17">
-        <v>4500</v>
+      <c r="E21" s="13">
+        <v>2250</v>
       </c>
       <c r="F21" s="19">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>2250</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I21" s="4">
         <v>45392</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D22" s="13">
         <v>1</v>
       </c>
       <c r="E22" s="13">
-        <v>2250</v>
+        <v>4500</v>
       </c>
       <c r="F22" s="19">
         <f t="shared" si="0"/>
-        <v>2250</v>
+        <v>4500</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="4">
+        <v>45392</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="13">
         <v>10</v>
       </c>
-      <c r="I22" s="4">
-        <v>45392</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="13">
-        <v>1</v>
-      </c>
-      <c r="E23" s="13">
-        <v>4500</v>
+      <c r="E23" s="17">
+        <v>6515</v>
       </c>
       <c r="F23" s="19">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>65150</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="I23" s="4">
         <v>45392</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="13">
+        <v>2</v>
+      </c>
+      <c r="E24" s="17">
+        <v>43125</v>
+      </c>
+      <c r="F24" s="19">
+        <f t="shared" si="0"/>
+        <v>86250</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="13">
-        <v>10</v>
-      </c>
-      <c r="E24" s="17">
-        <v>6515</v>
-      </c>
-      <c r="F24" s="19">
-        <f t="shared" si="0"/>
-        <v>65150</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I24" s="4">
         <v>45392</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="13">
+        <v>4</v>
+      </c>
+      <c r="E25" s="17">
+        <v>10785</v>
+      </c>
+      <c r="F25" s="19">
+        <f t="shared" si="0"/>
+        <v>43140</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="13">
-        <v>2</v>
-      </c>
-      <c r="E25" s="17">
-        <v>43125</v>
-      </c>
-      <c r="F25" s="19">
-        <f t="shared" si="0"/>
-        <v>86250</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I25" s="4">
         <v>45392</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="13">
+        <v>5</v>
+      </c>
+      <c r="E26" s="17">
+        <v>37375</v>
+      </c>
+      <c r="F26" s="19">
+        <f t="shared" si="0"/>
+        <v>186875</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="13">
-        <v>4</v>
-      </c>
-      <c r="E26" s="17">
-        <v>10785</v>
-      </c>
-      <c r="F26" s="19">
-        <f t="shared" si="0"/>
-        <v>43140</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I26" s="4">
         <v>45392</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D27" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E27" s="17">
-        <v>37375</v>
+        <v>21920</v>
       </c>
       <c r="F27" s="19">
         <f t="shared" si="0"/>
-        <v>186875</v>
+        <v>43840</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I27" s="4">
         <v>45392</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28" s="17">
-        <v>21920</v>
+        <v>1000</v>
       </c>
       <c r="F28" s="19">
         <f t="shared" si="0"/>
-        <v>43840</v>
+        <v>3000</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I28" s="4">
         <v>45392</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D29" s="13">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E29" s="17">
-        <v>1000</v>
+        <v>350</v>
       </c>
       <c r="F29" s="19">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>4200</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I29" s="4">
         <v>45392</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D30" s="13">
+        <v>36</v>
+      </c>
+      <c r="E30" s="17">
+        <v>2000</v>
+      </c>
+      <c r="F30" s="19">
+        <f t="shared" si="0"/>
+        <v>72000</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="17">
-        <v>350</v>
-      </c>
-      <c r="F30" s="19">
-        <f t="shared" si="0"/>
-        <v>4200</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I30" s="4">
         <v>45392</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D31" s="13">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E31" s="17">
-        <v>2000</v>
+        <v>8650</v>
       </c>
       <c r="F31" s="19">
         <f t="shared" si="0"/>
-        <v>72000</v>
+        <v>17300</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I31" s="4">
         <v>45392</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B32" s="2"/>
       <c r="C32" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D32" s="13">
-        <v>2</v>
-      </c>
-      <c r="E32" s="17">
-        <v>8650</v>
+        <v>1</v>
+      </c>
+      <c r="E32" s="16">
+        <v>46980</v>
       </c>
       <c r="F32" s="19">
         <f t="shared" si="0"/>
-        <v>17300</v>
+        <v>46980</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I32" s="4">
         <v>45392</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="5" t="s">
-        <v>8</v>
+      <c r="C33" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="D33" s="13">
-        <v>1</v>
-      </c>
-      <c r="E33" s="16">
-        <v>46980</v>
+        <v>60</v>
+      </c>
+      <c r="E33" s="13">
+        <v>230</v>
       </c>
       <c r="F33" s="19">
         <f t="shared" si="0"/>
-        <v>46980</v>
+        <v>13800</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I33" s="4">
         <v>45392</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D34" s="13">
         <v>60</v>
       </c>
       <c r="E34" s="13">
-        <v>230</v>
+        <v>120</v>
       </c>
       <c r="F34" s="19">
         <f t="shared" si="0"/>
-        <v>13800</v>
+        <v>7200</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I34" s="4">
         <v>45392</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D35" s="13">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E35" s="13">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="F35" s="19">
         <f t="shared" si="0"/>
-        <v>7200</v>
+        <v>6200</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I35" s="4">
         <v>45392</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D36" s="13">
         <v>40</v>
       </c>
       <c r="E36" s="13">
-        <v>155</v>
+        <v>250</v>
       </c>
       <c r="F36" s="19">
         <f t="shared" si="0"/>
-        <v>6200</v>
+        <v>10000</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I36" s="4">
         <v>45392</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="B37" s="5"/>
       <c r="C37" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D37" s="13">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E37" s="13">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="F37" s="19">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>400</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I37" s="4">
         <v>45392</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="B38" s="2"/>
       <c r="C38" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D38" s="13">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E38" s="13">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="F38" s="19">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>3600</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I38" s="4">
         <v>45392</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D39" s="13">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E39" s="13">
-        <v>120</v>
+        <v>1200</v>
       </c>
       <c r="F39" s="19">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I39" s="4">
         <v>45392</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="6" t="s">
@@ -1929,208 +1898,177 @@
         <v>1</v>
       </c>
       <c r="E40" s="13">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="F40" s="19">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I40" s="4">
         <v>45392</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="13">
+        <v>5</v>
+      </c>
+      <c r="E41" s="13">
+        <v>800</v>
+      </c>
+      <c r="F41" s="19">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="13">
-        <v>1</v>
-      </c>
-      <c r="E41" s="13">
-        <v>500</v>
-      </c>
-      <c r="F41" s="19">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="I41" s="4">
         <v>45392</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D42" s="13">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E42" s="13">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="F42" s="19">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I42" s="4">
         <v>45392</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D43" s="13">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E43" s="13">
-        <v>400</v>
+        <v>4000</v>
       </c>
       <c r="F43" s="19">
         <f t="shared" si="0"/>
         <v>8000</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I43" s="4">
         <v>45392</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B44" s="2"/>
-      <c r="C44" s="6" t="s">
-        <v>15</v>
+      <c r="C44" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="D44" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44" s="13">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="F44" s="19">
-        <f t="shared" si="0"/>
-        <v>8000</v>
+        <f>E44*D44</f>
+        <v>3000</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I44" s="4">
         <v>45392</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="7" t="s">
-        <v>6</v>
+      <c r="C45" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="D45" s="13">
         <v>1</v>
       </c>
       <c r="E45" s="13">
-        <v>3000</v>
-      </c>
-      <c r="F45" s="19">
-        <f>E45*D45</f>
-        <v>3000</v>
+        <v>80250</v>
+      </c>
+      <c r="F45" s="13">
+        <v>80250</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I45" s="4">
         <v>45392</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="13">
-        <v>1</v>
-      </c>
-      <c r="E46" s="13">
-        <v>80250</v>
-      </c>
-      <c r="F46" s="13">
-        <v>80250</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I46" s="4">
-        <v>45392</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>